<commit_message>
Began implementing system for code based text
Created individual files for each language to set the parameters of their text.
Began creating a system in intro.js so that text can be inserted from the associated language file with the correct styling.
</commit_message>
<xml_diff>
--- a/src/MonkeyRalley_TranslationPictureList.xlsx
+++ b/src/MonkeyRalley_TranslationPictureList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Taylor\Documents\MIIS\_2021_Fall\Software Internationalization\FinalProject_MonkeyGame\ludum-dare-28-master\Software-Internationalization_Final-Project_Monkey-Rally\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA13EAF0-4D5C-45CF-8C9C-7DB1603F29AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE5DD4E-0B0A-422D-8556-2DED03545498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97647C9A-1BFA-4474-A525-A5F09A9CEAA9}"/>
   </bookViews>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89CF139-094A-4567-B335-CDF415CD4ABF}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finalized it, both content and preloader; adjusted text due to text expansion
</commit_message>
<xml_diff>
--- a/src/MonkeyRalley_TranslationPictureList.xlsx
+++ b/src/MonkeyRalley_TranslationPictureList.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\GitHub\Software-Internationalization_Final-Project_Monkey-Rally\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738B609C-0A81-4B03-B5EC-EBDFB2C92344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="27420" windowHeight="12580"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="162">
   <si>
     <t>en</t>
   </si>
@@ -250,9 +256,6 @@
     <t>（*或者说这是一个神奇的故事，讲述了一只忠诚的小猴子是如何从大火和灾祸中将我拯救出来。）</t>
   </si>
   <si>
-    <t>( * o la fantastica storia di quella volta in cui mi sono stato salvato dalle fiamme e disavventure grazie all'aiuto di una fedele e leale scimmietta)</t>
-  </si>
-  <si>
     <t>私の友人の猿が火事の中で私を助けてくれたの素晴らしい物語！</t>
   </si>
   <si>
@@ -500,19 +503,16 @@
   </si>
   <si>
     <t>언어</t>
+  </si>
+  <si>
+    <t>( * o la fantastica storia di quella volta che mi sono salvato dalle fiamme e disavventure grazie all'aiuto di una fedele e leale scimmietta)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,152 +520,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,192 +530,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -867,251 +543,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1121,61 +555,17 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1433,30 +823,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="24.3359375" customWidth="1"/>
-    <col min="2" max="2" width="27.46875" customWidth="1"/>
-    <col min="3" max="3" width="27.3359375" customWidth="1"/>
-    <col min="4" max="5" width="27.46875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.46484375" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="5" width="27.46484375" customWidth="1"/>
     <col min="6" max="6" width="27.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="28" spans="1:6">
+    <row r="3" spans="1:6" ht="28.5">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1510,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="28.5">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1748,7 +1137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" ht="42" spans="1:6">
+    <row r="18" spans="1:6" ht="42.75">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -1756,265 +1145,265 @@
         <v>77</v>
       </c>
       <c r="D18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
         <v>78</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" t="s">
         <v>96</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>97</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" t="s">
         <v>101</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>102</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="D24" t="s">
         <v>106</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>107</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>112</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="D26" t="s">
         <v>116</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>117</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>122</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="D28" t="s">
         <v>126</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>127</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" t="s">
         <v>131</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>132</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" t="s">
         <v>136</v>
       </c>
-      <c r="D30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D31" t="s">
         <v>140</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>141</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="D32" t="s">
         <v>145</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>146</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="D33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" t="s">
         <v>150</v>
-      </c>
-      <c r="D33" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" t="s">
-        <v>151</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>75</v>
@@ -2022,40 +1411,39 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" t="s">
         <v>153</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>154</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" t="s">
         <v>158</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>159</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>161</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JA and ZH buttons
</commit_message>
<xml_diff>
--- a/src/MonkeyRalley_TranslationPictureList.xlsx
+++ b/src/MonkeyRalley_TranslationPictureList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\GitHub\Software-Internationalization_Final-Project_Monkey-Rally\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekaterinacudinova/Documents/GitHub/Software-Internationalization_Final-Project_Monkey-Rally/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738B609C-0A81-4B03-B5EC-EBDFB2C92344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBEBA66-CDCF-294E-932F-9086768946B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27420" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="193">
   <si>
     <t>en</t>
   </si>
@@ -256,6 +256,9 @@
     <t>（*或者说这是一个神奇的故事，讲述了一只忠诚的小猴子是如何从大火和灾祸中将我拯救出来。）</t>
   </si>
   <si>
+    <t>( * o la fantastica storia di quella volta in cui mi sono stato salvato dalle fiamme e disavventure grazie all'aiuto di una fedele e leale scimmietta)</t>
+  </si>
+  <si>
     <t>私の友人の猿が火事の中で私を助けてくれたの素晴らしい物語！</t>
   </si>
   <si>
@@ -505,19 +508,122 @@
     <t>언어</t>
   </si>
   <si>
-    <t>( * o la fantastica storia di quella volta che mi sono salvato dalle fiamme e disavventure grazie all'aiuto di una fedele e leale scimmietta)</t>
+    <t>Загрузка…</t>
+  </si>
+  <si>
+    <t>О нет! В лаборатории произошла авария и ты застряла в огне!</t>
+  </si>
+  <si>
+    <t>Твоя армия обученных обезьянок сбежала…</t>
+  </si>
+  <si>
+    <t>…все, кроме одной.</t>
+  </si>
+  <si>
+    <t>одной обезьянки.</t>
+  </si>
+  <si>
+    <t>дай ей инструкции,</t>
+  </si>
+  <si>
+    <t>чтобы спастись!</t>
+  </si>
+  <si>
+    <t>Авторы:</t>
+  </si>
+  <si>
+    <t>Код:</t>
+  </si>
+  <si>
+    <t>Иллюстрации:</t>
+  </si>
+  <si>
+    <t>Музыка:</t>
+  </si>
+  <si>
+    <t>Побег Обезьянок</t>
+  </si>
+  <si>
+    <t>Кликните, чтобы начать!</t>
+  </si>
+  <si>
+    <t>*или удивительная история о том, как я спаслась от пожара и катастрофы благодаря надежному и верному другу-обезьянке)</t>
+  </si>
+  <si>
+    <t>У тебя получилось!</t>
+  </si>
+  <si>
+    <t>Назад</t>
+  </si>
+  <si>
+    <t>авторы</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Уровень 8</t>
+  </si>
+  <si>
+    <t>меню</t>
+  </si>
+  <si>
+    <t>дальше</t>
+  </si>
+  <si>
+    <t>играть</t>
+  </si>
+  <si>
+    <t>выкл. звук</t>
+  </si>
+  <si>
+    <t>вкл. звук</t>
+  </si>
+  <si>
+    <t>язык</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -547,13 +653,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,21 +938,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.46484375" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="5" width="27.46484375" customWidth="1"/>
-    <col min="6" max="6" width="27.796875" customWidth="1"/>
+    <col min="4" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,13 +972,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
@@ -882,13 +992,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.5">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
@@ -899,13 +1012,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -916,13 +1032,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
@@ -933,13 +1052,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
@@ -950,13 +1072,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="D7" t="s">
         <v>33</v>
       </c>
@@ -967,13 +1092,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="D8" t="s">
         <v>38</v>
       </c>
@@ -984,13 +1112,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="D9" t="s">
         <v>43</v>
       </c>
@@ -1001,13 +1132,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
@@ -1018,13 +1152,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
       <c r="D11" t="s">
         <v>51</v>
       </c>
@@ -1035,13 +1172,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="D12" t="s">
         <v>55</v>
       </c>
@@ -1052,13 +1192,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
       <c r="D13" t="s">
         <v>58</v>
       </c>
@@ -1069,13 +1212,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="D14" t="s">
         <v>62</v>
       </c>
@@ -1086,13 +1232,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
       <c r="D15" t="s">
         <v>65</v>
       </c>
@@ -1103,13 +1252,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="C16" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
@@ -1120,13 +1272,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="D17" t="s">
         <v>73</v>
       </c>
@@ -1137,313 +1292,368 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="42.75">
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="C18" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C21" s="4" t="s">
+        <v>178</v>
+      </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" t="s">
         <v>135</v>
       </c>
-      <c r="D30" t="s">
-        <v>134</v>
-      </c>
       <c r="E30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" t="s">
         <v>149</v>
       </c>
-      <c r="D33" t="s">
-        <v>148</v>
-      </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>